<commit_message>
Add SPOTV ON, SPOTV ON2
</commit_message>
<xml_diff>
--- a/채널정보.xlsx
+++ b/채널정보.xlsx
@@ -2754,8 +2754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
-      <selection activeCell="G339" sqref="G339"/>
+    <sheetView tabSelected="1" topLeftCell="A304" workbookViewId="0">
+      <selection activeCell="G315" sqref="G315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>